<commit_message>
add auto color test case and fix auto color issue
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import2007.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="126">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>The row 10 - 11 is hidden</t>
+  </si>
+  <si>
+    <t>auto color</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="56">
+  <fonts count="57">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -821,6 +824,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1165,7 +1175,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1409,6 +1419,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1802,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1848,7 +1859,9 @@
       <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="155" t="s">
+        <v>125</v>
+      </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -2666,7 +2679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
export chart - area, bar, column, doughnut, line, pie, stock
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import2007.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -403,7 +403,7 @@
     <t>The row 10 - 11 is hidden</t>
   </si>
   <si>
-    <t>auto color</t>
+    <t>auto color font</t>
   </si>
 </sst>
 </file>
@@ -1396,6 +1396,7 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1419,7 +1420,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1859,7 +1859,7 @@
       <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="134" t="s">
         <v>125</v>
       </c>
       <c r="E2" s="11"/>
@@ -1876,17 +1876,17 @@
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
@@ -1959,17 +1959,17 @@
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="136" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
@@ -2629,11 +2629,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="81"/>
-      <c r="F2" s="136">
+      <c r="F2" s="137">
         <v>1</v>
       </c>
-      <c r="G2" s="137"/>
-      <c r="H2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="139"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="81"/>
@@ -2647,9 +2647,9 @@
         <v>6</v>
       </c>
       <c r="E3" s="81"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="141"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="142"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="81"/>
@@ -2836,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2845,6 +2845,7 @@
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21">
@@ -3321,16 +3322,16 @@
       <c r="A28" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="142" t="s">
+      <c r="B28" s="143" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="143"/>
+      <c r="C28" s="144"/>
       <c r="D28" s="94"/>
-      <c r="E28" s="142" t="s">
+      <c r="E28" s="143" t="s">
         <v>110</v>
       </c>
-      <c r="F28" s="144"/>
-      <c r="G28" s="143"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="144"/>
       <c r="H28" s="94"/>
       <c r="I28" s="94"/>
       <c r="J28" s="94"/>
@@ -3367,13 +3368,13 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="94"/>
-      <c r="B31" s="145" t="s">
+      <c r="B31" s="146" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="148" t="s">
+      <c r="C31" s="149" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="149"/>
+      <c r="D31" s="150"/>
       <c r="E31" s="94"/>
       <c r="F31" s="94"/>
       <c r="G31" s="94"/>
@@ -3385,9 +3386,9 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="94"/>
-      <c r="B32" s="146"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="151"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="151"/>
+      <c r="D32" s="152"/>
       <c r="E32" s="94"/>
       <c r="F32" s="94"/>
       <c r="G32" s="94"/>
@@ -3399,9 +3400,9 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="94"/>
-      <c r="B33" s="147"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="153"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="154"/>
       <c r="E33" s="94"/>
       <c r="F33" s="94"/>
       <c r="G33" s="94"/>
@@ -3534,13 +3535,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="155" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="129" t="s">

</xml_diff>